<commit_message>
Added curated set of Dp core promoter motifs and description table.
</commit_message>
<xml_diff>
--- a/promoter_analyses/Dm_core_motifs/Dm_motifs_table.xlsx
+++ b/promoter_analyses/Dm_core_motifs/Dm_motifs_table.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="24620" yWindow="11860" windowWidth="26540" windowHeight="15280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -379,8 +379,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -400,17 +404,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -743,7 +751,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -787,252 +795,252 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3">
-        <v>253</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F3" s="2"/>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="E4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4">
-        <v>252</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2"/>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="F5">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C7" s="2"/>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F7">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>37</v>
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8">
+        <v>251</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="F9">
+        <v>253</v>
+      </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C12" s="2"/>
       <c r="E12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="2"/>
+        <v>50</v>
+      </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C13" s="2"/>
       <c r="E13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C14" s="2"/>
       <c r="E14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="E15" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>57</v>
+        <v>36</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
+        <v>56</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="E16" t="s">
+        <v>49</v>
       </c>
       <c r="F16">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="G16" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="7:7">
@@ -1056,8 +1064,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B3:G15">
-    <sortCondition descending="1" ref="F3:F15"/>
+  <sortState ref="A3:G16">
+    <sortCondition ref="A3:A16"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>